<commit_message>
website update without landing page updates
</commit_message>
<xml_diff>
--- a/content/species/data/sp_fwf_tbl_2.xlsx
+++ b/content/species/data/sp_fwf_tbl_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_repos\species\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B6E625-3C52-4DEC-8C2A-9CE59FCC8A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F366B4-0282-4268-A37B-384615834288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{434242FF-20E2-45EF-9689-865BD324F483}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{434242FF-20E2-45EF-9689-865BD324F483}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
-  <si>
-    <t>Taxon name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Endemism</t>
   </si>
@@ -50,9 +47,6 @@
     <t>[*Brycinus lateralis*] (https://speciesstatus.sanbi.org/assessment/last-assessment/162/)</t>
   </si>
   <si>
-    <t>Brycinus lateralis</t>
-  </si>
-  <si>
     <t>Not-endemic</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
     <t>[*Chiloglanis bifurcus*]\* (https://speciesstatus.sanbi.org/assessment/last-assessment/56/)</t>
   </si>
   <si>
-    <t>Chiloglanis bifurcus</t>
-  </si>
-  <si>
     <t>Endemic</t>
   </si>
   <si>
@@ -83,9 +74,6 @@
     <t>[*Chiloglanis emarginatus*]\* (https://speciesstatus.sanbi.org/taxa/list/?search=Chiloglanis+emarginatus)</t>
   </si>
   <si>
-    <t>Chiloglanis emarginatus</t>
-  </si>
-  <si>
     <t>NT to VU</t>
   </si>
   <si>
@@ -95,9 +83,6 @@
     <t>[*Ctenopoma multispine*] (https://speciesstatus.sanbi.org/assessment/last-assessment/176/)</t>
   </si>
   <si>
-    <t>Ctenopoma multispine</t>
-  </si>
-  <si>
     <t>LC to VU</t>
   </si>
   <si>
@@ -107,24 +92,15 @@
     <t>[*Enteromius gurneyi*]\* (https://speciesstatus.sanbi.org/assessment/last-assessment/80/)</t>
   </si>
   <si>
-    <t>Enteromius gurneyi</t>
-  </si>
-  <si>
     <t>Agriculture &amp; aquaculture, Climate change &amp; severe weather, Invasive and other problematic species, Pollution, Residential &amp; commercial development.</t>
   </si>
   <si>
     <t>[*Enteromius lineomaculatus*] (https://speciesstatus.sanbi.org/assessment/last-assessment/167/)</t>
   </si>
   <si>
-    <t>Enteromius lineomaculatus</t>
-  </si>
-  <si>
     <t>Agriculture &amp; aquaculture. Pollution.</t>
   </si>
   <si>
-    <t>Micropanchax myaposae</t>
-  </si>
-  <si>
     <t>Near-endemic</t>
   </si>
   <si>
@@ -132,9 +108,6 @@
   </si>
   <si>
     <t>[*Oreochromis mossambicus*] (https://speciesstatus.sanbi.org/assessment/last-assessment/26/)</t>
-  </si>
-  <si>
-    <t>Oreochromis mossambicus</t>
   </si>
   <si>
     <t>Invasive and other problematic species.</t>
@@ -156,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,18 +138,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF242424"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -196,22 +161,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -544,238 +506,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3131CE09-1F12-425F-A08B-F76532EF677F}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="65" customWidth="1"/>
-    <col min="2" max="4" width="24.44140625" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.41796875" customWidth="1"/>
+    <col min="4" max="4" width="19.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>34</v>
-      </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>36</v>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
+      <c r="E7" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="E9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{8A6F5E17-1801-4948-8E38-7717B520BC28}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{3917E639-1A78-4D86-8C42-79C8539E1A05}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{868531C2-9E63-4D6A-92B0-ECF2CD418911}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{98D8CE39-2FA8-4225-88C5-B02B304F7B70}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{BBF2D3DD-56F4-41C1-ACDE-E0991F19E6E9}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{C34C4176-F50E-4F71-99D7-EE20CC9A5C44}"/>
-    <hyperlink ref="B3" r:id="rId7" xr:uid="{7BF557D4-790F-46D1-9FA0-60AD5394D502}"/>
-    <hyperlink ref="B2" r:id="rId8" xr:uid="{C31FE514-9E62-4C2E-9154-C8EDD11DA396}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d08e37f2-beba-4595-a3e8-aa91f032b3fc" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de6781d5-cbdf-44cc-b8b1-919d4413b058">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9251B87A2689245AA9FD86C69F20C58" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a4ec884e7468e8b6decba7ff9ee350d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de6781d5-cbdf-44cc-b8b1-919d4413b058" xmlns:ns3="d08e37f2-beba-4595-a3e8-aa91f032b3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b02cf9d369237c4b82eaa1e33230624f" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1047,27 +950,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B34CC-3D18-4FF9-88B0-794D32A5F1E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d08e37f2-beba-4595-a3e8-aa91f032b3fc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de6781d5-cbdf-44cc-b8b1-919d4413b058"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{782A8BF3-702A-4EB3-B088-9466AB7713F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d08e37f2-beba-4595-a3e8-aa91f032b3fc" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de6781d5-cbdf-44cc-b8b1-919d4413b058">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EAD6FB9-CE22-4602-B9C9-65F6A6B46EB0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1085,4 +990,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{782A8BF3-702A-4EB3-B088-9466AB7713F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B34CC-3D18-4FF9-88B0-794D32A5F1E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d08e37f2-beba-4595-a3e8-aa91f032b3fc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de6781d5-cbdf-44cc-b8b1-919d4413b058"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>